<commit_message>
Financial Institute Creation and validations
</commit_message>
<xml_diff>
--- a/hostID_Automation_withTestNG/TestData/TestData_HostID.xlsx
+++ b/hostID_Automation_withTestNG/TestData/TestData_HostID.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13365" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Financial_Institution" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>edit_Initials</t>
   </si>
@@ -37,6 +38,66 @@
   </si>
   <si>
     <t>correctNetworkPassword</t>
+  </si>
+  <si>
+    <t>Institution_Name</t>
+  </si>
+  <si>
+    <t>FI_Number</t>
+  </si>
+  <si>
+    <t>Address_Line1</t>
+  </si>
+  <si>
+    <t>Address_Line2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>ZIP_SUFFIX</t>
+  </si>
+  <si>
+    <t>Corporate_Structure</t>
+  </si>
+  <si>
+    <t>TAX_Identification_Number</t>
+  </si>
+  <si>
+    <t>OmniBus_Account_Number</t>
+  </si>
+  <si>
+    <t>Special_Instructions</t>
+  </si>
+  <si>
+    <t>Omni_Serve</t>
+  </si>
+  <si>
+    <t>NSCC_ID</t>
+  </si>
+  <si>
+    <t>SuccessMessage_FailureMessage</t>
+  </si>
+  <si>
+    <t>MessageKeyword</t>
+  </si>
+  <si>
+    <t>AccountExist</t>
+  </si>
+  <si>
+    <t>WrongTaxIdNumber</t>
+  </si>
+  <si>
+    <t>WrongNSCCID</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
 </sst>
 </file>
@@ -377,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -436,12 +497,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>